<commit_message>
included csv and xlsx files as well as some new R code
</commit_message>
<xml_diff>
--- a/SWFWMD/Van Fleet 2 623026 and 623033.xlsx
+++ b/SWFWMD/Van Fleet 2 623026 and 623033.xlsx
@@ -8,17 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ad.sfwmd.gov\dfsroot\data\wsd\SUP\proj\CFWI_WetlandStress\Update2018\SWFWMD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F909103D-98AD-475D-9AEA-9BFDD3D2A21E}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D75E66BC-5B71-4983-9F8C-17A44E1FA7A0}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="623026" sheetId="1" r:id="rId1"/>
+    <sheet name="POLK COUNTY VF-2MW" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'623026'!$A$1:$N$248</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'POLK COUNTY VF-2MW'!$A$1:$N$248</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="179021"/>
 </workbook>
 </file>
 
@@ -924,7 +924,7 @@
   <dimension ref="A1:N262"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E254" sqref="E254"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>